<commit_message>
SDGS-76 indicators sheet added to results
</commit_message>
<xml_diff>
--- a/keywords/indicators.xlsx
+++ b/keywords/indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67CB32E-17FC-4DF0-A1E3-AB7D48B816BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B1AEC8-81EE-412F-B414-A74508D457DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="362">
   <si>
     <t>Goal</t>
   </si>
@@ -90,564 +90,6 @@
     <t>SDG 9</t>
   </si>
   <si>
-    <t>Target 1.0</t>
-  </si>
-  <si>
-    <t>Target 1.1</t>
-  </si>
-  <si>
-    <t>Target 1.2</t>
-  </si>
-  <si>
-    <t>Target 1.3</t>
-  </si>
-  <si>
-    <t>Target 1.4</t>
-  </si>
-  <si>
-    <t>Target 1.5</t>
-  </si>
-  <si>
-    <t>Target 1.a</t>
-  </si>
-  <si>
-    <t>Target 1.b</t>
-  </si>
-  <si>
-    <t>Target 10.0</t>
-  </si>
-  <si>
-    <t>Target 10.1</t>
-  </si>
-  <si>
-    <t>Target 10.2</t>
-  </si>
-  <si>
-    <t>Target 10.3</t>
-  </si>
-  <si>
-    <t>Target 10.4</t>
-  </si>
-  <si>
-    <t>Target 10.5</t>
-  </si>
-  <si>
-    <t>Target 10.6</t>
-  </si>
-  <si>
-    <t>Target 10.7</t>
-  </si>
-  <si>
-    <t>Target 10.a</t>
-  </si>
-  <si>
-    <t>Target 10.b</t>
-  </si>
-  <si>
-    <t>Target 10.c</t>
-  </si>
-  <si>
-    <t>Target 11.0</t>
-  </si>
-  <si>
-    <t>Target 11.1</t>
-  </si>
-  <si>
-    <t>Target 11.2</t>
-  </si>
-  <si>
-    <t>Target 11.3</t>
-  </si>
-  <si>
-    <t>Target 11.4</t>
-  </si>
-  <si>
-    <t>Target 11.5</t>
-  </si>
-  <si>
-    <t>Target 11.6</t>
-  </si>
-  <si>
-    <t>Target 11.7</t>
-  </si>
-  <si>
-    <t>Target 11.a</t>
-  </si>
-  <si>
-    <t>Target 11.b</t>
-  </si>
-  <si>
-    <t>Target 11.c</t>
-  </si>
-  <si>
-    <t>Target 12.0</t>
-  </si>
-  <si>
-    <t>Target 12.1</t>
-  </si>
-  <si>
-    <t>Target 12.2</t>
-  </si>
-  <si>
-    <t>Target 12.3</t>
-  </si>
-  <si>
-    <t>Target 12.4</t>
-  </si>
-  <si>
-    <t>Target 12.5</t>
-  </si>
-  <si>
-    <t>Target 12.6</t>
-  </si>
-  <si>
-    <t>Target 12.7</t>
-  </si>
-  <si>
-    <t>Target 12.8</t>
-  </si>
-  <si>
-    <t>Target 12.a</t>
-  </si>
-  <si>
-    <t>Target 12.b</t>
-  </si>
-  <si>
-    <t>Target 12.c</t>
-  </si>
-  <si>
-    <t>Target 13.0</t>
-  </si>
-  <si>
-    <t>Target 13.1</t>
-  </si>
-  <si>
-    <t>Target 13.2</t>
-  </si>
-  <si>
-    <t>Target 13.3</t>
-  </si>
-  <si>
-    <t>Target 13.a</t>
-  </si>
-  <si>
-    <t>Target 13.b</t>
-  </si>
-  <si>
-    <t>Target 14.0</t>
-  </si>
-  <si>
-    <t>Target 14.1</t>
-  </si>
-  <si>
-    <t>Target 14.2</t>
-  </si>
-  <si>
-    <t>Target 14.3</t>
-  </si>
-  <si>
-    <t>Target 14.4</t>
-  </si>
-  <si>
-    <t>Target 14.5</t>
-  </si>
-  <si>
-    <t>Target 14.6</t>
-  </si>
-  <si>
-    <t>Target 14.7</t>
-  </si>
-  <si>
-    <t>Target 14.a</t>
-  </si>
-  <si>
-    <t>Target 14.b</t>
-  </si>
-  <si>
-    <t>Target 14.c</t>
-  </si>
-  <si>
-    <t>Target 15.0</t>
-  </si>
-  <si>
-    <t>Target 15.1</t>
-  </si>
-  <si>
-    <t>Target 15.2</t>
-  </si>
-  <si>
-    <t>Target 15.3</t>
-  </si>
-  <si>
-    <t>Target 15.4</t>
-  </si>
-  <si>
-    <t>Target 15.5</t>
-  </si>
-  <si>
-    <t>Target 15.6</t>
-  </si>
-  <si>
-    <t>Target 15.7</t>
-  </si>
-  <si>
-    <t>Target 15.8</t>
-  </si>
-  <si>
-    <t>Target 15.9</t>
-  </si>
-  <si>
-    <t>Target 15.a</t>
-  </si>
-  <si>
-    <t>Target 15.b</t>
-  </si>
-  <si>
-    <t>Target 15.c</t>
-  </si>
-  <si>
-    <t>Target 16.0</t>
-  </si>
-  <si>
-    <t>Target 16.1</t>
-  </si>
-  <si>
-    <t>Target 16.10</t>
-  </si>
-  <si>
-    <t>Target 16.2</t>
-  </si>
-  <si>
-    <t>Target 16.3</t>
-  </si>
-  <si>
-    <t>Target 16.4</t>
-  </si>
-  <si>
-    <t>Target 16.5</t>
-  </si>
-  <si>
-    <t>Target 16.6</t>
-  </si>
-  <si>
-    <t>Target 16.7</t>
-  </si>
-  <si>
-    <t>Target 16.8</t>
-  </si>
-  <si>
-    <t>Target 16.9</t>
-  </si>
-  <si>
-    <t>Target 16.a</t>
-  </si>
-  <si>
-    <t>Target 16.b</t>
-  </si>
-  <si>
-    <t>Target 17.0</t>
-  </si>
-  <si>
-    <t>Target 17.1</t>
-  </si>
-  <si>
-    <t>Target 17.10</t>
-  </si>
-  <si>
-    <t>Target 17.11</t>
-  </si>
-  <si>
-    <t>Target 17.12</t>
-  </si>
-  <si>
-    <t>Target 17.13</t>
-  </si>
-  <si>
-    <t>Target 17.14</t>
-  </si>
-  <si>
-    <t>Target 17.15</t>
-  </si>
-  <si>
-    <t>Target 17.16</t>
-  </si>
-  <si>
-    <t>Target 17.17</t>
-  </si>
-  <si>
-    <t>Target 17.18</t>
-  </si>
-  <si>
-    <t>Target 17.19</t>
-  </si>
-  <si>
-    <t>Target 17.2</t>
-  </si>
-  <si>
-    <t>Target 17.3</t>
-  </si>
-  <si>
-    <t>Target 17.4</t>
-  </si>
-  <si>
-    <t>Target 17.5</t>
-  </si>
-  <si>
-    <t>Target 17.6</t>
-  </si>
-  <si>
-    <t>Target 17.7</t>
-  </si>
-  <si>
-    <t>Target 17.8</t>
-  </si>
-  <si>
-    <t>Target 17.9</t>
-  </si>
-  <si>
-    <t>Target 2.0</t>
-  </si>
-  <si>
-    <t>Target 2.1</t>
-  </si>
-  <si>
-    <t>Target 2.2</t>
-  </si>
-  <si>
-    <t>Target 2.3</t>
-  </si>
-  <si>
-    <t>Target 2.4</t>
-  </si>
-  <si>
-    <t>Target 2.5</t>
-  </si>
-  <si>
-    <t>Target 2.a</t>
-  </si>
-  <si>
-    <t>Target 2.b</t>
-  </si>
-  <si>
-    <t>Target 2.c</t>
-  </si>
-  <si>
-    <t>Target 3.0</t>
-  </si>
-  <si>
-    <t>Target 3.1</t>
-  </si>
-  <si>
-    <t>Target 3.2</t>
-  </si>
-  <si>
-    <t>Target 3.3</t>
-  </si>
-  <si>
-    <t>Target 3.4</t>
-  </si>
-  <si>
-    <t>Target 3.5</t>
-  </si>
-  <si>
-    <t>Target 3.6</t>
-  </si>
-  <si>
-    <t>Target 3.7</t>
-  </si>
-  <si>
-    <t>Target 3.8</t>
-  </si>
-  <si>
-    <t>Target 3.9</t>
-  </si>
-  <si>
-    <t>Target 3.a</t>
-  </si>
-  <si>
-    <t>Target 3.b</t>
-  </si>
-  <si>
-    <t>Target 3.c</t>
-  </si>
-  <si>
-    <t>Target 3.d</t>
-  </si>
-  <si>
-    <t>Target 4.0</t>
-  </si>
-  <si>
-    <t>Target 4.1</t>
-  </si>
-  <si>
-    <t>Target 4.2</t>
-  </si>
-  <si>
-    <t>Target 4.3</t>
-  </si>
-  <si>
-    <t>Target 4.4</t>
-  </si>
-  <si>
-    <t>Target 4.5</t>
-  </si>
-  <si>
-    <t>Target 4.6</t>
-  </si>
-  <si>
-    <t>Target 4.7</t>
-  </si>
-  <si>
-    <t>Target 4.a</t>
-  </si>
-  <si>
-    <t>Target 4.b</t>
-  </si>
-  <si>
-    <t>Target 4.c</t>
-  </si>
-  <si>
-    <t>Target 5.0</t>
-  </si>
-  <si>
-    <t>Target 5.1</t>
-  </si>
-  <si>
-    <t>Target 5.2</t>
-  </si>
-  <si>
-    <t>Target 5.3</t>
-  </si>
-  <si>
-    <t>Target 5.4</t>
-  </si>
-  <si>
-    <t>Target 5.5</t>
-  </si>
-  <si>
-    <t>Target 5.6</t>
-  </si>
-  <si>
-    <t>Target 5.a</t>
-  </si>
-  <si>
-    <t>Target 5.b</t>
-  </si>
-  <si>
-    <t>Target 5.c</t>
-  </si>
-  <si>
-    <t>Target 6.0</t>
-  </si>
-  <si>
-    <t>Target 6.1</t>
-  </si>
-  <si>
-    <t>Target 6.2</t>
-  </si>
-  <si>
-    <t>Target 6.3</t>
-  </si>
-  <si>
-    <t>Target 6.4</t>
-  </si>
-  <si>
-    <t>Target 6.5</t>
-  </si>
-  <si>
-    <t>Target 6.6</t>
-  </si>
-  <si>
-    <t>Target 6.a</t>
-  </si>
-  <si>
-    <t>Target 6.b</t>
-  </si>
-  <si>
-    <t>Target 7.0</t>
-  </si>
-  <si>
-    <t>Target 7.1</t>
-  </si>
-  <si>
-    <t>Target 7.2</t>
-  </si>
-  <si>
-    <t>Target 7.3</t>
-  </si>
-  <si>
-    <t>Target 7.a</t>
-  </si>
-  <si>
-    <t>Target 7.b</t>
-  </si>
-  <si>
-    <t>Target 8.0</t>
-  </si>
-  <si>
-    <t>Target 8.1</t>
-  </si>
-  <si>
-    <t>Target 8.10</t>
-  </si>
-  <si>
-    <t>Target 8.2</t>
-  </si>
-  <si>
-    <t>Target 8.3</t>
-  </si>
-  <si>
-    <t>Target 8.4</t>
-  </si>
-  <si>
-    <t>Target 8.5</t>
-  </si>
-  <si>
-    <t>Target 8.6</t>
-  </si>
-  <si>
-    <t>Target 8.7</t>
-  </si>
-  <si>
-    <t>Target 8.8</t>
-  </si>
-  <si>
-    <t>Target 8.9</t>
-  </si>
-  <si>
-    <t>Target 8.a</t>
-  </si>
-  <si>
-    <t>Target 8.b</t>
-  </si>
-  <si>
-    <t>Target 9.0</t>
-  </si>
-  <si>
-    <t>Target 9.1</t>
-  </si>
-  <si>
-    <t>Target 9.2</t>
-  </si>
-  <si>
-    <t>Target 9.3</t>
-  </si>
-  <si>
-    <t>Target 9.4</t>
-  </si>
-  <si>
-    <t>Target 9.5</t>
-  </si>
-  <si>
-    <t>Target 9.a</t>
-  </si>
-  <si>
-    <t>Target 9.b</t>
-  </si>
-  <si>
-    <t>Target 9.c</t>
-  </si>
-  <si>
     <t>1.1.1</t>
   </si>
   <si>
@@ -1153,6 +595,528 @@
   </si>
   <si>
     <t>UN Indicators</t>
+  </si>
+  <si>
+    <t>1.a</t>
+  </si>
+  <si>
+    <t>1.b</t>
+  </si>
+  <si>
+    <t>2.a</t>
+  </si>
+  <si>
+    <t>2.b</t>
+  </si>
+  <si>
+    <t>2.c</t>
+  </si>
+  <si>
+    <t>3.a</t>
+  </si>
+  <si>
+    <t>3.b</t>
+  </si>
+  <si>
+    <t>3.c</t>
+  </si>
+  <si>
+    <t>3.d</t>
+  </si>
+  <si>
+    <t>4.a</t>
+  </si>
+  <si>
+    <t>4.b</t>
+  </si>
+  <si>
+    <t>4.c</t>
+  </si>
+  <si>
+    <t>5.a</t>
+  </si>
+  <si>
+    <t>5.b</t>
+  </si>
+  <si>
+    <t>5.c</t>
+  </si>
+  <si>
+    <t>6.a</t>
+  </si>
+  <si>
+    <t>6.b</t>
+  </si>
+  <si>
+    <t>7.a</t>
+  </si>
+  <si>
+    <t>7.b</t>
+  </si>
+  <si>
+    <t>8.a</t>
+  </si>
+  <si>
+    <t>8.b</t>
+  </si>
+  <si>
+    <t>9.a</t>
+  </si>
+  <si>
+    <t>9.b</t>
+  </si>
+  <si>
+    <t>9.c</t>
+  </si>
+  <si>
+    <t>10.a</t>
+  </si>
+  <si>
+    <t>10.b</t>
+  </si>
+  <si>
+    <t>10.c</t>
+  </si>
+  <si>
+    <t>11.a</t>
+  </si>
+  <si>
+    <t>11.b</t>
+  </si>
+  <si>
+    <t>11.c</t>
+  </si>
+  <si>
+    <t>12.a</t>
+  </si>
+  <si>
+    <t>12.b</t>
+  </si>
+  <si>
+    <t>12.c</t>
+  </si>
+  <si>
+    <t>13.a</t>
+  </si>
+  <si>
+    <t>13.b</t>
+  </si>
+  <si>
+    <t>14.a</t>
+  </si>
+  <si>
+    <t>14.b</t>
+  </si>
+  <si>
+    <t>14.c</t>
+  </si>
+  <si>
+    <t>15.a</t>
+  </si>
+  <si>
+    <t>15.b</t>
+  </si>
+  <si>
+    <t>15.c</t>
+  </si>
+  <si>
+    <t>16.a</t>
+  </si>
+  <si>
+    <t>16.b</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>10.7</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>11.5</t>
+  </si>
+  <si>
+    <t>11.6</t>
+  </si>
+  <si>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>12.7</t>
+  </si>
+  <si>
+    <t>12.8</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>14.3</t>
+  </si>
+  <si>
+    <t>14.4</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>14.6</t>
+  </si>
+  <si>
+    <t>14.7</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>15.3</t>
+  </si>
+  <si>
+    <t>15.4</t>
+  </si>
+  <si>
+    <t>15.5</t>
+  </si>
+  <si>
+    <t>15.6</t>
+  </si>
+  <si>
+    <t>15.7</t>
+  </si>
+  <si>
+    <t>15.8</t>
+  </si>
+  <si>
+    <t>15.9</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>16.2</t>
+  </si>
+  <si>
+    <t>16.3</t>
+  </si>
+  <si>
+    <t>16.4</t>
+  </si>
+  <si>
+    <t>16.5</t>
+  </si>
+  <si>
+    <t>16.6</t>
+  </si>
+  <si>
+    <t>16.7</t>
+  </si>
+  <si>
+    <t>16.8</t>
+  </si>
+  <si>
+    <t>16.9</t>
+  </si>
+  <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.2</t>
+  </si>
+  <si>
+    <t>17.3</t>
+  </si>
+  <si>
+    <t>17.4</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>17.6</t>
+  </si>
+  <si>
+    <t>17.7</t>
+  </si>
+  <si>
+    <t>17.8</t>
+  </si>
+  <si>
+    <t>17.9</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1537,7 +1502,7 @@
   <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C187"/>
+      <selection activeCell="B2" sqref="B2:B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,2003 +1515,2003 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>373</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
+      <c r="B2" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
+      <c r="B3" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
+      <c r="B4" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
+      <c r="B5" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
+      <c r="B6" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
+      <c r="B7" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
+      <c r="B8" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="C8" t="s">
-        <v>210</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
+      <c r="B9" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>124</v>
+      <c r="B10" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>125</v>
+      <c r="B11" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="C11" t="s">
-        <v>300</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>126</v>
+      <c r="B12" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="C12" t="s">
-        <v>301</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>127</v>
+      <c r="B13" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="C13" t="s">
-        <v>302</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>128</v>
+      <c r="B14" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C14" t="s">
-        <v>303</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>129</v>
+      <c r="B15" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>130</v>
+      <c r="B16" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>305</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
-        <v>131</v>
+      <c r="B17" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="C17" t="s">
-        <v>306</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
-        <v>132</v>
+      <c r="B18" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>133</v>
+      <c r="B19" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
-        <v>134</v>
+      <c r="B20" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="C20" t="s">
-        <v>308</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
-        <v>135</v>
+      <c r="B21" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="C21" t="s">
-        <v>309</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
-        <v>136</v>
+      <c r="B22" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="C22" t="s">
-        <v>310</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
-        <v>137</v>
+      <c r="B23" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="C23" t="s">
-        <v>311</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
-        <v>138</v>
+      <c r="B24" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="C24" t="s">
-        <v>312</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
-        <v>139</v>
+      <c r="B25" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="C25" t="s">
-        <v>313</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>140</v>
+      <c r="B26" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="C26" t="s">
-        <v>314</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>141</v>
+      <c r="B27" s="1" t="s">
+        <v>251</v>
       </c>
       <c r="C27" t="s">
-        <v>315</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
-        <v>142</v>
+      <c r="B28" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="C28" t="s">
-        <v>316</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29" t="s">
-        <v>143</v>
+      <c r="B29" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="C29" t="s">
-        <v>317</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
-        <v>144</v>
+      <c r="B30" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="C30" t="s">
-        <v>318</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" t="s">
-        <v>145</v>
+      <c r="B31" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="C31" t="s">
-        <v>319</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
-        <v>146</v>
+      <c r="B32" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="C32" t="s">
-        <v>320</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
-        <v>147</v>
+      <c r="B33" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" t="s">
-        <v>148</v>
+      <c r="B34" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="C34" t="s">
-        <v>321</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
-        <v>149</v>
+      <c r="B35" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="C35" t="s">
-        <v>322</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36" t="s">
-        <v>150</v>
+      <c r="B36" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="C36" t="s">
-        <v>323</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
-      <c r="B37" t="s">
-        <v>151</v>
+      <c r="B37" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="C37" t="s">
-        <v>324</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
-        <v>152</v>
+      <c r="B38" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="C38" t="s">
-        <v>325</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39" t="s">
-        <v>153</v>
+      <c r="B39" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="C39" t="s">
-        <v>326</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B40" t="s">
-        <v>154</v>
+      <c r="B40" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="C40" t="s">
-        <v>327</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B41" t="s">
-        <v>155</v>
+      <c r="B41" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>328</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42" t="s">
-        <v>156</v>
+      <c r="B42" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="C42" t="s">
-        <v>329</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
-        <v>157</v>
+      <c r="B43" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="C43" t="s">
-        <v>330</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
-        <v>158</v>
+      <c r="B44" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
-      <c r="B45" t="s">
-        <v>159</v>
+      <c r="B45" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="C45" t="s">
-        <v>331</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B46" t="s">
-        <v>160</v>
+      <c r="B46" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="C46" t="s">
-        <v>332</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
-        <v>161</v>
+      <c r="B47" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="C47" t="s">
-        <v>333</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
-      <c r="B48" t="s">
-        <v>162</v>
+      <c r="B48" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="C48" t="s">
-        <v>334</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>14</v>
       </c>
-      <c r="B49" t="s">
-        <v>163</v>
+      <c r="B49" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="C49" t="s">
-        <v>335</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
-      <c r="B50" t="s">
-        <v>164</v>
+      <c r="B50" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="C50" t="s">
-        <v>336</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
-      <c r="B51" t="s">
-        <v>165</v>
+      <c r="B51" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="C51" t="s">
-        <v>337</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
-      <c r="B52" t="s">
-        <v>166</v>
+      <c r="B52" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>338</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
-      <c r="B53" t="s">
-        <v>167</v>
+      <c r="B53" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="C53" t="s">
-        <v>339</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
-      <c r="B54" t="s">
-        <v>168</v>
+      <c r="B54" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
-      <c r="B55" t="s">
-        <v>169</v>
+      <c r="B55" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="C55" t="s">
-        <v>340</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
-      <c r="B56" t="s">
-        <v>170</v>
+      <c r="B56" s="1" t="s">
+        <v>270</v>
       </c>
       <c r="C56" t="s">
-        <v>341</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
-      <c r="B57" t="s">
-        <v>171</v>
+      <c r="B57" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="C57" t="s">
-        <v>342</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
-      <c r="B58" t="s">
-        <v>172</v>
+      <c r="B58" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C58" t="s">
-        <v>343</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
-      <c r="B59" t="s">
-        <v>173</v>
+      <c r="B59" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="C59" t="s">
-        <v>344</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
-      <c r="B60" t="s">
-        <v>174</v>
+      <c r="B60" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="C60" t="s">
-        <v>345</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>15</v>
       </c>
-      <c r="B61" t="s">
-        <v>175</v>
+      <c r="B61" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="C61" t="s">
-        <v>346</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
-      <c r="B62" t="s">
-        <v>176</v>
+      <c r="B62" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="C62" t="s">
-        <v>347</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
-      <c r="B63" t="s">
-        <v>177</v>
+      <c r="B63" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
-      <c r="B64" t="s">
-        <v>178</v>
+      <c r="B64" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="C64" t="s">
-        <v>348</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
-      <c r="B65" t="s">
-        <v>179</v>
+      <c r="B65" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="C65" t="s">
-        <v>349</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
-      <c r="B66" t="s">
-        <v>180</v>
+      <c r="B66" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="C66" t="s">
-        <v>350</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
-      <c r="B67" t="s">
-        <v>181</v>
+      <c r="B67" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="C67" t="s">
-        <v>351</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
-      <c r="B68" t="s">
-        <v>182</v>
+      <c r="B68" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>352</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>17</v>
       </c>
-      <c r="B69" t="s">
-        <v>183</v>
+      <c r="B69" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>184</v>
+      <c r="B70" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="C70" t="s">
-        <v>353</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
-      <c r="B71" t="s">
-        <v>185</v>
+      <c r="B71" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="C71" t="s">
-        <v>354</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>17</v>
       </c>
-      <c r="B72" t="s">
-        <v>186</v>
+      <c r="B72" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="C72" t="s">
-        <v>355</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>17</v>
       </c>
-      <c r="B73" t="s">
-        <v>187</v>
+      <c r="B73" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="C73" t="s">
-        <v>356</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>17</v>
       </c>
-      <c r="B74" t="s">
-        <v>188</v>
+      <c r="B74" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="C74" t="s">
-        <v>357</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>17</v>
       </c>
-      <c r="B75" t="s">
-        <v>189</v>
+      <c r="B75" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="C75" t="s">
-        <v>358</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
-      <c r="B76" t="s">
-        <v>190</v>
+      <c r="B76" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="C76" t="s">
-        <v>359</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>17</v>
       </c>
-      <c r="B77" t="s">
-        <v>191</v>
+      <c r="B77" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="C77" t="s">
-        <v>360</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>17</v>
       </c>
-      <c r="B78" t="s">
-        <v>192</v>
+      <c r="B78" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C78" t="s">
-        <v>361</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>17</v>
       </c>
-      <c r="B79" t="s">
-        <v>193</v>
+      <c r="B79" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="C79" t="s">
-        <v>362</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>17</v>
       </c>
-      <c r="B80" t="s">
-        <v>194</v>
+      <c r="B80" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="C80" t="s">
-        <v>363</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>17</v>
       </c>
-      <c r="B81" t="s">
-        <v>195</v>
+      <c r="B81" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="C81" t="s">
-        <v>364</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>18</v>
       </c>
-      <c r="B82" t="s">
-        <v>196</v>
+      <c r="B82" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>18</v>
       </c>
-      <c r="B83" t="s">
-        <v>197</v>
+      <c r="B83" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="C83" t="s">
-        <v>365</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>18</v>
       </c>
-      <c r="B84" t="s">
-        <v>198</v>
+      <c r="B84" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="C84" t="s">
-        <v>366</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>18</v>
       </c>
-      <c r="B85" t="s">
-        <v>199</v>
+      <c r="B85" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="C85" t="s">
-        <v>367</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>18</v>
       </c>
-      <c r="B86" t="s">
-        <v>200</v>
+      <c r="B86" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="C86" t="s">
-        <v>368</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>18</v>
       </c>
-      <c r="B87" t="s">
-        <v>201</v>
+      <c r="B87" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="C87" t="s">
-        <v>369</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>18</v>
       </c>
-      <c r="B88" t="s">
-        <v>202</v>
+      <c r="B88" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="C88" t="s">
-        <v>370</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>18</v>
       </c>
-      <c r="B89" t="s">
-        <v>203</v>
+      <c r="B89" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="C89" t="s">
-        <v>371</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>18</v>
       </c>
-      <c r="B90" t="s">
-        <v>204</v>
+      <c r="B90" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="C90" t="s">
-        <v>372</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>3</v>
       </c>
-      <c r="B91" t="s">
-        <v>27</v>
+      <c r="B91" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>3</v>
       </c>
-      <c r="B92" t="s">
-        <v>28</v>
+      <c r="B92" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="C92" t="s">
-        <v>212</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>3</v>
       </c>
-      <c r="B93" t="s">
-        <v>29</v>
+      <c r="B93" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="C93" t="s">
-        <v>213</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>3</v>
       </c>
-      <c r="B94" t="s">
-        <v>30</v>
+      <c r="B94" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="C94" t="s">
-        <v>214</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>3</v>
       </c>
-      <c r="B95" t="s">
-        <v>31</v>
+      <c r="B95" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="C95" t="s">
-        <v>215</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>3</v>
       </c>
-      <c r="B96" t="s">
-        <v>32</v>
+      <c r="B96" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="C96" t="s">
-        <v>216</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
-      <c r="B97" t="s">
-        <v>33</v>
+      <c r="B97" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="C97" t="s">
-        <v>217</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
-      <c r="B98" t="s">
-        <v>34</v>
+      <c r="B98" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C98" t="s">
-        <v>218</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
-      <c r="B99" t="s">
-        <v>35</v>
+      <c r="B99" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="C99" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
-      <c r="B100" t="s">
-        <v>36</v>
+      <c r="B100" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="C100" t="s">
-        <v>220</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>3</v>
       </c>
-      <c r="B101" t="s">
-        <v>37</v>
+      <c r="B101" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="C101" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4</v>
       </c>
-      <c r="B102" t="s">
-        <v>38</v>
+      <c r="B102" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>4</v>
       </c>
-      <c r="B103" t="s">
-        <v>39</v>
+      <c r="B103" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="C103" t="s">
-        <v>222</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>4</v>
       </c>
-      <c r="B104" t="s">
-        <v>40</v>
+      <c r="B104" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>223</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>4</v>
       </c>
-      <c r="B105" t="s">
-        <v>41</v>
+      <c r="B105" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="C105" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>4</v>
       </c>
-      <c r="B106" t="s">
-        <v>42</v>
+      <c r="B106" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="C106" t="s">
-        <v>225</v>
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>4</v>
       </c>
-      <c r="B107" t="s">
-        <v>43</v>
+      <c r="B107" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="C107" t="s">
-        <v>226</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>4</v>
       </c>
-      <c r="B108" t="s">
-        <v>44</v>
+      <c r="B108" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="C108" t="s">
-        <v>227</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>4</v>
       </c>
-      <c r="B109" t="s">
-        <v>45</v>
+      <c r="B109" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="C109" t="s">
-        <v>228</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>4</v>
       </c>
-      <c r="B110" t="s">
-        <v>46</v>
+      <c r="B110" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>43</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>4</v>
       </c>
-      <c r="B111" t="s">
-        <v>47</v>
+      <c r="B111" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C111" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>4</v>
       </c>
-      <c r="B112" t="s">
-        <v>48</v>
+      <c r="B112" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>5</v>
       </c>
-      <c r="B113" t="s">
-        <v>49</v>
+      <c r="B113" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>5</v>
       </c>
-      <c r="B114" t="s">
-        <v>50</v>
+      <c r="B114" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="C114" t="s">
-        <v>231</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>5</v>
       </c>
-      <c r="B115" t="s">
-        <v>51</v>
+      <c r="B115" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="C115" t="s">
-        <v>232</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>5</v>
       </c>
-      <c r="B116" t="s">
-        <v>52</v>
+      <c r="B116" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="C116" t="s">
-        <v>233</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>5</v>
       </c>
-      <c r="B117" t="s">
-        <v>53</v>
+      <c r="B117" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>5</v>
       </c>
-      <c r="B118" t="s">
-        <v>54</v>
+      <c r="B118" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>5</v>
       </c>
-      <c r="B119" t="s">
-        <v>55</v>
+      <c r="B119" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="C119" t="s">
-        <v>236</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>5</v>
       </c>
-      <c r="B120" t="s">
-        <v>56</v>
+      <c r="B120" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="C120" t="s">
-        <v>237</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>5</v>
       </c>
-      <c r="B121" t="s">
-        <v>57</v>
+      <c r="B121" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="C121" t="s">
-        <v>238</v>
+        <v>52</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>5</v>
       </c>
-      <c r="B122" t="s">
-        <v>58</v>
+      <c r="B122" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C122" t="s">
-        <v>239</v>
+        <v>53</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>5</v>
       </c>
-      <c r="B123" t="s">
-        <v>59</v>
+      <c r="B123" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="C123" t="s">
-        <v>240</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>5</v>
       </c>
-      <c r="B124" t="s">
-        <v>60</v>
+      <c r="B124" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="C124" t="s">
-        <v>241</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>6</v>
       </c>
-      <c r="B125" t="s">
-        <v>61</v>
+      <c r="B125" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
-      <c r="B126" t="s">
-        <v>62</v>
+      <c r="B126" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="C126" t="s">
-        <v>242</v>
+        <v>56</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>6</v>
       </c>
-      <c r="B127" t="s">
-        <v>63</v>
+      <c r="B127" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C127" t="s">
-        <v>243</v>
+        <v>57</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>6</v>
       </c>
-      <c r="B128" t="s">
-        <v>64</v>
+      <c r="B128" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="C128" t="s">
-        <v>244</v>
+        <v>58</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>6</v>
       </c>
-      <c r="B129" t="s">
-        <v>65</v>
+      <c r="B129" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="C129" t="s">
-        <v>245</v>
+        <v>59</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>6</v>
       </c>
-      <c r="B130" t="s">
-        <v>66</v>
+      <c r="B130" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="C130" t="s">
-        <v>246</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
-      <c r="B131" t="s">
-        <v>67</v>
+      <c r="B131" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>7</v>
       </c>
-      <c r="B132" t="s">
-        <v>68</v>
+      <c r="B132" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="C132" t="s">
-        <v>247</v>
+        <v>61</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>7</v>
       </c>
-      <c r="B133" t="s">
-        <v>69</v>
+      <c r="B133" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="C133" t="s">
-        <v>248</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>7</v>
       </c>
-      <c r="B134" t="s">
-        <v>70</v>
+      <c r="B134" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="C134" t="s">
-        <v>249</v>
+        <v>63</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>7</v>
       </c>
-      <c r="B135" t="s">
-        <v>71</v>
+      <c r="B135" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C135" t="s">
-        <v>250</v>
+        <v>64</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>7</v>
       </c>
-      <c r="B136" t="s">
-        <v>72</v>
+      <c r="B136" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="C136" t="s">
-        <v>251</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>7</v>
       </c>
-      <c r="B137" t="s">
-        <v>73</v>
+      <c r="B137" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="C137" t="s">
-        <v>252</v>
+        <v>66</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>7</v>
       </c>
-      <c r="B138" t="s">
-        <v>74</v>
+      <c r="B138" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="C138" t="s">
-        <v>253</v>
+        <v>67</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>7</v>
       </c>
-      <c r="B139" t="s">
-        <v>75</v>
+      <c r="B139" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="C139" t="s">
-        <v>254</v>
+        <v>68</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>7</v>
       </c>
-      <c r="B140" t="s">
-        <v>76</v>
+      <c r="B140" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="C140" t="s">
-        <v>255</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>7</v>
       </c>
-      <c r="B141" t="s">
-        <v>77</v>
+      <c r="B141" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="C141" t="s">
-        <v>256</v>
+        <v>70</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>8</v>
       </c>
-      <c r="B142" t="s">
-        <v>78</v>
+      <c r="B142" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>8</v>
       </c>
-      <c r="B143" t="s">
-        <v>79</v>
+      <c r="B143" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="C143" t="s">
-        <v>257</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>8</v>
       </c>
-      <c r="B144" t="s">
-        <v>80</v>
+      <c r="B144" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="C144" t="s">
-        <v>258</v>
+        <v>72</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>8</v>
       </c>
-      <c r="B145" t="s">
-        <v>81</v>
+      <c r="B145" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="C145" t="s">
-        <v>259</v>
+        <v>73</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>8</v>
       </c>
-      <c r="B146" t="s">
-        <v>82</v>
+      <c r="B146" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="C146" t="s">
-        <v>260</v>
+        <v>74</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>8</v>
       </c>
-      <c r="B147" t="s">
-        <v>83</v>
+      <c r="B147" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="C147" t="s">
-        <v>261</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>8</v>
       </c>
-      <c r="B148" t="s">
-        <v>84</v>
+      <c r="B148" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="C148" t="s">
-        <v>262</v>
+        <v>76</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>8</v>
       </c>
-      <c r="B149" t="s">
-        <v>85</v>
+      <c r="B149" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="C149" t="s">
-        <v>263</v>
+        <v>77</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>8</v>
       </c>
-      <c r="B150" t="s">
-        <v>86</v>
+      <c r="B150" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="C150" t="s">
-        <v>264</v>
+        <v>78</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>8</v>
       </c>
-      <c r="B151" t="s">
-        <v>87</v>
+      <c r="B151" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="C151" t="s">
-        <v>265</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>8</v>
       </c>
-      <c r="B152" t="s">
-        <v>88</v>
+      <c r="B152" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="C152" t="s">
-        <v>266</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>8</v>
       </c>
-      <c r="B153" t="s">
-        <v>89</v>
+      <c r="B153" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="C153" t="s">
-        <v>267</v>
+        <v>81</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>8</v>
       </c>
-      <c r="B154" t="s">
-        <v>90</v>
+      <c r="B154" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C154" t="s">
-        <v>268</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>9</v>
       </c>
-      <c r="B155" t="s">
-        <v>91</v>
+      <c r="B155" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
-      <c r="B156" t="s">
-        <v>92</v>
+      <c r="B156" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="C156" t="s">
-        <v>269</v>
+        <v>83</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
-      <c r="B157" t="s">
-        <v>93</v>
+      <c r="B157" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="C157" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
-      <c r="B158" t="s">
-        <v>94</v>
+      <c r="B158" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="C158" t="s">
-        <v>271</v>
+        <v>85</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>9</v>
       </c>
-      <c r="B159" t="s">
-        <v>95</v>
+      <c r="B159" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="C159" t="s">
-        <v>272</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>9</v>
       </c>
-      <c r="B160" t="s">
-        <v>96</v>
+      <c r="B160" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="C160" t="s">
-        <v>273</v>
+        <v>87</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>9</v>
       </c>
-      <c r="B161" t="s">
-        <v>97</v>
+      <c r="B161" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="C161" t="s">
-        <v>274</v>
+        <v>88</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>9</v>
       </c>
-      <c r="B162" t="s">
-        <v>98</v>
+      <c r="B162" s="1" t="s">
+        <v>348</v>
       </c>
       <c r="C162" t="s">
-        <v>275</v>
+        <v>89</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
-      <c r="B163" t="s">
-        <v>99</v>
+      <c r="B163" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="C163" t="s">
-        <v>276</v>
+        <v>90</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
-      <c r="B164" t="s">
-        <v>100</v>
+      <c r="B164" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="C164" t="s">
-        <v>277</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
-      <c r="B165" t="s">
-        <v>101</v>
+      <c r="B165" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="C165" t="s">
-        <v>278</v>
+        <v>92</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>9</v>
       </c>
-      <c r="B166" t="s">
-        <v>102</v>
+      <c r="B166" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="C166" t="s">
-        <v>279</v>
+        <v>93</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
-      <c r="B167" t="s">
-        <v>103</v>
+      <c r="B167" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="C167" t="s">
-        <v>280</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>10</v>
       </c>
-      <c r="B168" t="s">
-        <v>104</v>
+      <c r="B168" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>10</v>
       </c>
-      <c r="B169" t="s">
-        <v>105</v>
+      <c r="B169" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C169" t="s">
-        <v>281</v>
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>10</v>
       </c>
-      <c r="B170" t="s">
-        <v>106</v>
+      <c r="B170" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C170" t="s">
-        <v>282</v>
+        <v>96</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>10</v>
       </c>
-      <c r="B171" t="s">
-        <v>107</v>
+      <c r="B171" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C171" t="s">
-        <v>283</v>
+        <v>97</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>10</v>
       </c>
-      <c r="B172" t="s">
-        <v>108</v>
+      <c r="B172" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C172" t="s">
-        <v>284</v>
+        <v>98</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>10</v>
       </c>
-      <c r="B173" t="s">
-        <v>109</v>
+      <c r="B173" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C173" t="s">
-        <v>285</v>
+        <v>99</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>10</v>
       </c>
-      <c r="B174" t="s">
-        <v>110</v>
+      <c r="B174" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C174" t="s">
-        <v>286</v>
+        <v>100</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>10</v>
       </c>
-      <c r="B175" t="s">
-        <v>111</v>
+      <c r="B175" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C175" t="s">
-        <v>287</v>
+        <v>101</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>10</v>
       </c>
-      <c r="B176" t="s">
-        <v>112</v>
+      <c r="B176" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C176" t="s">
-        <v>288</v>
+        <v>102</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>10</v>
       </c>
-      <c r="B177" t="s">
-        <v>113</v>
+      <c r="B177" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C177" t="s">
-        <v>289</v>
+        <v>103</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>10</v>
       </c>
-      <c r="B178" t="s">
-        <v>114</v>
+      <c r="B178" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C178" t="s">
-        <v>290</v>
+        <v>104</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>10</v>
       </c>
-      <c r="B179" t="s">
-        <v>115</v>
+      <c r="B179" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C179" t="s">
-        <v>291</v>
+        <v>105</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>10</v>
       </c>
-      <c r="B180" t="s">
-        <v>116</v>
+      <c r="B180" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C180" t="s">
-        <v>292</v>
+        <v>106</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>10</v>
       </c>
-      <c r="B181" t="s">
-        <v>117</v>
+      <c r="B181" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="C181" t="s">
-        <v>293</v>
+        <v>107</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>10</v>
       </c>
-      <c r="B182" t="s">
-        <v>118</v>
+      <c r="B182" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="C182" t="s">
-        <v>294</v>
+        <v>108</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>10</v>
       </c>
-      <c r="B183" t="s">
-        <v>119</v>
+      <c r="B183" s="1" t="s">
+        <v>357</v>
       </c>
       <c r="C183" t="s">
-        <v>295</v>
+        <v>109</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>10</v>
       </c>
-      <c r="B184" t="s">
-        <v>120</v>
+      <c r="B184" s="1" t="s">
+        <v>358</v>
       </c>
       <c r="C184" t="s">
-        <v>296</v>
+        <v>110</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>10</v>
       </c>
-      <c r="B185" t="s">
-        <v>121</v>
+      <c r="B185" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="C185" t="s">
-        <v>297</v>
+        <v>111</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>10</v>
       </c>
-      <c r="B186" t="s">
-        <v>122</v>
+      <c r="B186" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="C186" t="s">
-        <v>298</v>
+        <v>112</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>10</v>
       </c>
-      <c r="B187" t="s">
-        <v>123</v>
+      <c r="B187" s="1" t="s">
+        <v>361</v>
       </c>
       <c r="C187" t="s">
-        <v>299</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SDGS-76 prototype of indicators.json creating function, some fixing required in the main script to append the indicators in the excel files as string instead of lists
</commit_message>
<xml_diff>
--- a/keywords/indicators.xlsx
+++ b/keywords/indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B1AEC8-81EE-412F-B414-A74508D457DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7400AAF-4B80-45E0-9105-8827EEC3AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="374">
   <si>
     <t>Goal</t>
   </si>
@@ -90,513 +90,6 @@
     <t>SDG 9</t>
   </si>
   <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
-    <t>1.2.1, 1.2.2</t>
-  </si>
-  <si>
-    <t>1.3.1</t>
-  </si>
-  <si>
-    <t>1.4.1, 1.4.2</t>
-  </si>
-  <si>
-    <t>1.5.1, 1.5.2, 1.5.3, 1.5.4</t>
-  </si>
-  <si>
-    <t>1.a.1, 1.a.2</t>
-  </si>
-  <si>
-    <t>1.b.1</t>
-  </si>
-  <si>
-    <t>10.1.1</t>
-  </si>
-  <si>
-    <t>10.2.1</t>
-  </si>
-  <si>
-    <t>10.3.1</t>
-  </si>
-  <si>
-    <t>10.4.1, 10.4.2</t>
-  </si>
-  <si>
-    <t>10.5.1</t>
-  </si>
-  <si>
-    <t>10.6.1</t>
-  </si>
-  <si>
-    <t>10.7.1, 10.7.2, 10.7.3, 10.7.4</t>
-  </si>
-  <si>
-    <t>10.a.1</t>
-  </si>
-  <si>
-    <t>10.b.1</t>
-  </si>
-  <si>
-    <t>10.c.1</t>
-  </si>
-  <si>
-    <t>11.1.1</t>
-  </si>
-  <si>
-    <t>11.2.1</t>
-  </si>
-  <si>
-    <t>11.3.1, 11.3.2</t>
-  </si>
-  <si>
-    <t>11.4.1</t>
-  </si>
-  <si>
-    <t>11.5.1, 11.5.2</t>
-  </si>
-  <si>
-    <t>11.6.1, 11.6.2</t>
-  </si>
-  <si>
-    <t>11.7.1, 11.7.2</t>
-  </si>
-  <si>
-    <t>11.a.1</t>
-  </si>
-  <si>
-    <t>11.b.1, 11.b.2</t>
-  </si>
-  <si>
-    <t>12.1.1</t>
-  </si>
-  <si>
-    <t>12.2.1, 12.2.2</t>
-  </si>
-  <si>
-    <t>12.3.1</t>
-  </si>
-  <si>
-    <t>12.4.1, 12.4.2</t>
-  </si>
-  <si>
-    <t>12.5.1</t>
-  </si>
-  <si>
-    <t>12.6.1</t>
-  </si>
-  <si>
-    <t>12.7.1</t>
-  </si>
-  <si>
-    <t>12.8.1</t>
-  </si>
-  <si>
-    <t>12.a.1</t>
-  </si>
-  <si>
-    <t>12.b.1</t>
-  </si>
-  <si>
-    <t>12.c.1</t>
-  </si>
-  <si>
-    <t>13.1.1, 13.1.2, 13.1.3</t>
-  </si>
-  <si>
-    <t>13.2.1, 13.2.2</t>
-  </si>
-  <si>
-    <t>13.3.1</t>
-  </si>
-  <si>
-    <t>13.a.1</t>
-  </si>
-  <si>
-    <t>13.b.1</t>
-  </si>
-  <si>
-    <t>14.1.1</t>
-  </si>
-  <si>
-    <t>14.2.1</t>
-  </si>
-  <si>
-    <t>14.3.1</t>
-  </si>
-  <si>
-    <t>14.4.1</t>
-  </si>
-  <si>
-    <t>14.5.1</t>
-  </si>
-  <si>
-    <t>14.6.1</t>
-  </si>
-  <si>
-    <t>14.7.1</t>
-  </si>
-  <si>
-    <t>14.a.1</t>
-  </si>
-  <si>
-    <t>14.b.1</t>
-  </si>
-  <si>
-    <t>14.c.1</t>
-  </si>
-  <si>
-    <t>15.1.1, 15.1.2</t>
-  </si>
-  <si>
-    <t>15.2.1</t>
-  </si>
-  <si>
-    <t>15.3.1</t>
-  </si>
-  <si>
-    <t>15.4.1, 15.4.2</t>
-  </si>
-  <si>
-    <t>15.5.1</t>
-  </si>
-  <si>
-    <t>15.6.1</t>
-  </si>
-  <si>
-    <t>15.7.1</t>
-  </si>
-  <si>
-    <t>15.8.1</t>
-  </si>
-  <si>
-    <t>15.9.1</t>
-  </si>
-  <si>
-    <t>15.a.1</t>
-  </si>
-  <si>
-    <t>15.b.1</t>
-  </si>
-  <si>
-    <t>15.c.1</t>
-  </si>
-  <si>
-    <t>16.1.1, 16.1.2, 16.1.3, 16.1.4</t>
-  </si>
-  <si>
-    <t>16.10.1, 16.10.2</t>
-  </si>
-  <si>
-    <t>16.2.1, 16.2.2, 16.2.3</t>
-  </si>
-  <si>
-    <t>16.3.1, 16.3.2, 16.3.3</t>
-  </si>
-  <si>
-    <t>16.4.1, 16.4.2</t>
-  </si>
-  <si>
-    <t>16.5.1, 16.5.2</t>
-  </si>
-  <si>
-    <t>16.6.1, 16.6.2</t>
-  </si>
-  <si>
-    <t>16.7.1, 16.7.2</t>
-  </si>
-  <si>
-    <t>16.8.1</t>
-  </si>
-  <si>
-    <t>16.9.1</t>
-  </si>
-  <si>
-    <t>16.a.1</t>
-  </si>
-  <si>
-    <t>16.b.1</t>
-  </si>
-  <si>
-    <t>17.1.1, 17.1.2</t>
-  </si>
-  <si>
-    <t>17.10.1</t>
-  </si>
-  <si>
-    <t>17.11.1</t>
-  </si>
-  <si>
-    <t>17.12.1</t>
-  </si>
-  <si>
-    <t>17.13.1</t>
-  </si>
-  <si>
-    <t>17.14.1</t>
-  </si>
-  <si>
-    <t>17.15.1</t>
-  </si>
-  <si>
-    <t>17.16.1</t>
-  </si>
-  <si>
-    <t>17.17.1</t>
-  </si>
-  <si>
-    <t>17.18.1, 17.18.2, 17.18.3</t>
-  </si>
-  <si>
-    <t>17.19.1, 17.19.2</t>
-  </si>
-  <si>
-    <t>17.2.1</t>
-  </si>
-  <si>
-    <t>17.3.1, 17.3.2</t>
-  </si>
-  <si>
-    <t>17.4.1</t>
-  </si>
-  <si>
-    <t>17.5.1</t>
-  </si>
-  <si>
-    <t>17.6.1</t>
-  </si>
-  <si>
-    <t>17.7.1</t>
-  </si>
-  <si>
-    <t>17.8.1</t>
-  </si>
-  <si>
-    <t>17.9.1</t>
-  </si>
-  <si>
-    <t>2.1.1, 2.1.2</t>
-  </si>
-  <si>
-    <t>2.2.1, 2.2.2, 2.2.3</t>
-  </si>
-  <si>
-    <t>2.3.1, 2.3.2</t>
-  </si>
-  <si>
-    <t>2.4.1</t>
-  </si>
-  <si>
-    <t>2.5.1, 2.5.2</t>
-  </si>
-  <si>
-    <t>2.a.1, 2.a.2</t>
-  </si>
-  <si>
-    <t>2.b.1</t>
-  </si>
-  <si>
-    <t>2.c.1</t>
-  </si>
-  <si>
-    <t>3.1.1, 3.1.2</t>
-  </si>
-  <si>
-    <t>3.2.1, 3.2.2</t>
-  </si>
-  <si>
-    <t>3.3.1, 3.3.2, 3.3.3, 3.3.4, 3.3.5</t>
-  </si>
-  <si>
-    <t>3.4.1, 3.4.2</t>
-  </si>
-  <si>
-    <t>3.5.1, 3.5.2</t>
-  </si>
-  <si>
-    <t>3.6.1</t>
-  </si>
-  <si>
-    <t>3.7.1, 3.7.2</t>
-  </si>
-  <si>
-    <t>3.8.1, 3.8.2</t>
-  </si>
-  <si>
-    <t>3.9.1, 3.9.2, 3.9.3</t>
-  </si>
-  <si>
-    <t>3.a.1</t>
-  </si>
-  <si>
-    <t>3.b.1, 3.b.2, 3.b.3</t>
-  </si>
-  <si>
-    <t>3.c.1</t>
-  </si>
-  <si>
-    <t>3.d.1, 3.d.2</t>
-  </si>
-  <si>
-    <t>4.1.1, 4.1.2</t>
-  </si>
-  <si>
-    <t>4.2.1, 4.2.2</t>
-  </si>
-  <si>
-    <t>4.3.1</t>
-  </si>
-  <si>
-    <t>4.4.1</t>
-  </si>
-  <si>
-    <t>4.5.1</t>
-  </si>
-  <si>
-    <t>4.6.1</t>
-  </si>
-  <si>
-    <t>4.7.1</t>
-  </si>
-  <si>
-    <t>4.a.1</t>
-  </si>
-  <si>
-    <t>4.b.1</t>
-  </si>
-  <si>
-    <t>4.c.1</t>
-  </si>
-  <si>
-    <t>5.1.1</t>
-  </si>
-  <si>
-    <t>5.2.1, 5.2.2</t>
-  </si>
-  <si>
-    <t>5.3.1, 5.3.2</t>
-  </si>
-  <si>
-    <t>5.4.1</t>
-  </si>
-  <si>
-    <t>5.5.1, 5.5.2</t>
-  </si>
-  <si>
-    <t>5.6.1, 5.6.2</t>
-  </si>
-  <si>
-    <t>5.a.1, 5.a.2</t>
-  </si>
-  <si>
-    <t>5.b.1</t>
-  </si>
-  <si>
-    <t>5.c.1</t>
-  </si>
-  <si>
-    <t>6.1.1</t>
-  </si>
-  <si>
-    <t>6.2.1</t>
-  </si>
-  <si>
-    <t>6.3.1, 6.3.2</t>
-  </si>
-  <si>
-    <t>6.4.1, 6.4.2</t>
-  </si>
-  <si>
-    <t>6.5.1, 6.5.2</t>
-  </si>
-  <si>
-    <t>6.6.1</t>
-  </si>
-  <si>
-    <t>6.a.1</t>
-  </si>
-  <si>
-    <t>6.b.1</t>
-  </si>
-  <si>
-    <t>7.1.1, 7.1.2</t>
-  </si>
-  <si>
-    <t>7.2.1</t>
-  </si>
-  <si>
-    <t>7.3.1</t>
-  </si>
-  <si>
-    <t>7.a.1</t>
-  </si>
-  <si>
-    <t>7.b.1</t>
-  </si>
-  <si>
-    <t>8.1.1</t>
-  </si>
-  <si>
-    <t>8.10.1, 8.10.2</t>
-  </si>
-  <si>
-    <t>8.2.1</t>
-  </si>
-  <si>
-    <t>8.3.1</t>
-  </si>
-  <si>
-    <t>8.4.1, 8.4.2</t>
-  </si>
-  <si>
-    <t>8.5.1, 8.5.2</t>
-  </si>
-  <si>
-    <t>8.6.1</t>
-  </si>
-  <si>
-    <t>8.7.1</t>
-  </si>
-  <si>
-    <t>8.8.1, 8.8.2</t>
-  </si>
-  <si>
-    <t>8.9.1</t>
-  </si>
-  <si>
-    <t>8.a.1</t>
-  </si>
-  <si>
-    <t>8.b.1</t>
-  </si>
-  <si>
-    <t>9.1.1, 9.1.2</t>
-  </si>
-  <si>
-    <t>9.2.1, 9.2.2</t>
-  </si>
-  <si>
-    <t>9.3.1, 9.3.2</t>
-  </si>
-  <si>
-    <t>9.4.1</t>
-  </si>
-  <si>
-    <t>9.5.1, 9.5.2</t>
-  </si>
-  <si>
-    <t>9.a.1</t>
-  </si>
-  <si>
-    <t>9.b.1</t>
-  </si>
-  <si>
-    <t>9.c.1</t>
-  </si>
-  <si>
-    <t>UN Indicators</t>
-  </si>
-  <si>
     <t>1.a</t>
   </si>
   <si>
@@ -1117,6 +610,549 @@
   </si>
   <si>
     <t>17.9</t>
+  </si>
+  <si>
+    <t>UN_Indicators</t>
+  </si>
+  <si>
+    <t>['']</t>
+  </si>
+  <si>
+    <t>['1.1.1']</t>
+  </si>
+  <si>
+    <t>['1.2.1', '1.2.2']</t>
+  </si>
+  <si>
+    <t>['1.3.1']</t>
+  </si>
+  <si>
+    <t>['1.4.1', '1.4.2']</t>
+  </si>
+  <si>
+    <t>['1.5.1', '1.5.2', '1.5.3', '1.5.4']</t>
+  </si>
+  <si>
+    <t>['1.a.1', '1.a.2']</t>
+  </si>
+  <si>
+    <t>['1.b.1']</t>
+  </si>
+  <si>
+    <t>['2.1.1', '2.1.2']</t>
+  </si>
+  <si>
+    <t>['2.2.1', '2.2.2', '2.2.3']</t>
+  </si>
+  <si>
+    <t>['2.3.1', '2.3.2']</t>
+  </si>
+  <si>
+    <t>['2.4.1']</t>
+  </si>
+  <si>
+    <t>['2.5.1', '2.5.2']</t>
+  </si>
+  <si>
+    <t>['2.a.1', '2.a.2']</t>
+  </si>
+  <si>
+    <t>['2.b.1']</t>
+  </si>
+  <si>
+    <t>['2.c.1']</t>
+  </si>
+  <si>
+    <t>['3.1.1', '3.1.2']</t>
+  </si>
+  <si>
+    <t>['3.2.1', '3.2.2']</t>
+  </si>
+  <si>
+    <t>['3.3.1', '3.3.2', '3.3.3', '3.3.4', '3.3.5']</t>
+  </si>
+  <si>
+    <t>['3.4.1', '3.4.2']</t>
+  </si>
+  <si>
+    <t>['3.5.1', '3.5.2']</t>
+  </si>
+  <si>
+    <t>['3.6.1']</t>
+  </si>
+  <si>
+    <t>['3.7.1', '3.7.2']</t>
+  </si>
+  <si>
+    <t>['3.8.1', '3.8.2']</t>
+  </si>
+  <si>
+    <t>['3.9.1', '3.9.2', '3.9.3']</t>
+  </si>
+  <si>
+    <t>['3.a.1']</t>
+  </si>
+  <si>
+    <t>['3.b.1', '3.b.2', '3.b.3']</t>
+  </si>
+  <si>
+    <t>['3.c.1']</t>
+  </si>
+  <si>
+    <t>['3.d.1', '3.d.2']</t>
+  </si>
+  <si>
+    <t>['4.1.1', '4.1.2']</t>
+  </si>
+  <si>
+    <t>['4.2.1', '4.2.2']</t>
+  </si>
+  <si>
+    <t>['4.3.1']</t>
+  </si>
+  <si>
+    <t>['4.4.1']</t>
+  </si>
+  <si>
+    <t>['4.5.1']</t>
+  </si>
+  <si>
+    <t>['4.6.1']</t>
+  </si>
+  <si>
+    <t>['4.7.1']</t>
+  </si>
+  <si>
+    <t>['4.a.1']</t>
+  </si>
+  <si>
+    <t>['4.b.1']</t>
+  </si>
+  <si>
+    <t>['4.c.1']</t>
+  </si>
+  <si>
+    <t>['5.1.1']</t>
+  </si>
+  <si>
+    <t>['5.2.1', '5.2.2']</t>
+  </si>
+  <si>
+    <t>['5.3.1', '5.3.2']</t>
+  </si>
+  <si>
+    <t>['5.4.1']</t>
+  </si>
+  <si>
+    <t>['5.5.1', '5.5.2']</t>
+  </si>
+  <si>
+    <t>['5.6.1', '5.6.2']</t>
+  </si>
+  <si>
+    <t>['5.a.1', '5.a.2']</t>
+  </si>
+  <si>
+    <t>['5.b.1']</t>
+  </si>
+  <si>
+    <t>['5.c.1']</t>
+  </si>
+  <si>
+    <t>['6.1.1']</t>
+  </si>
+  <si>
+    <t>['6.2.1']</t>
+  </si>
+  <si>
+    <t>['6.3.1', '6.3.2']</t>
+  </si>
+  <si>
+    <t>['6.4.1', '6.4.2']</t>
+  </si>
+  <si>
+    <t>['6.5.1', '6.5.2']</t>
+  </si>
+  <si>
+    <t>['6.6.1']</t>
+  </si>
+  <si>
+    <t>['6.a.1']</t>
+  </si>
+  <si>
+    <t>['6.b.1']</t>
+  </si>
+  <si>
+    <t>['7.1.1', '7.1.2']</t>
+  </si>
+  <si>
+    <t>['7.2.1']</t>
+  </si>
+  <si>
+    <t>['7.3.1']</t>
+  </si>
+  <si>
+    <t>['7.a.1']</t>
+  </si>
+  <si>
+    <t>['7.b.1']</t>
+  </si>
+  <si>
+    <t>['8.1.1']</t>
+  </si>
+  <si>
+    <t>['8.10.1', '8.10.2']</t>
+  </si>
+  <si>
+    <t>['8.2.1']</t>
+  </si>
+  <si>
+    <t>['8.3.1']</t>
+  </si>
+  <si>
+    <t>['8.4.1', '8.4.2']</t>
+  </si>
+  <si>
+    <t>['8.5.1', '8.5.2']</t>
+  </si>
+  <si>
+    <t>['8.6.1']</t>
+  </si>
+  <si>
+    <t>['8.7.1']</t>
+  </si>
+  <si>
+    <t>['8.8.1', '8.8.2']</t>
+  </si>
+  <si>
+    <t>['8.9.1']</t>
+  </si>
+  <si>
+    <t>['8.a.1']</t>
+  </si>
+  <si>
+    <t>['8.b.1']</t>
+  </si>
+  <si>
+    <t>['9.1.1', '9.1.2']</t>
+  </si>
+  <si>
+    <t>['9.2.1', '9.2.2']</t>
+  </si>
+  <si>
+    <t>['9.3.1', '9.3.2']</t>
+  </si>
+  <si>
+    <t>['9.4.1']</t>
+  </si>
+  <si>
+    <t>['9.5.1', '9.5.2']</t>
+  </si>
+  <si>
+    <t>['9.a.1']</t>
+  </si>
+  <si>
+    <t>['9.b.1']</t>
+  </si>
+  <si>
+    <t>['9.c.1']</t>
+  </si>
+  <si>
+    <t>['10.1.1']</t>
+  </si>
+  <si>
+    <t>['10.2.1']</t>
+  </si>
+  <si>
+    <t>['10.3.1']</t>
+  </si>
+  <si>
+    <t>['10.4.1', '10.4.2']</t>
+  </si>
+  <si>
+    <t>['10.5.1']</t>
+  </si>
+  <si>
+    <t>['10.6.1']</t>
+  </si>
+  <si>
+    <t>['10.7.1', '10.7.2', '10.7.3', '10.7.4']</t>
+  </si>
+  <si>
+    <t>['10.a.1']</t>
+  </si>
+  <si>
+    <t>['10.b.1']</t>
+  </si>
+  <si>
+    <t>['10.c.1']</t>
+  </si>
+  <si>
+    <t>['11.1.1']</t>
+  </si>
+  <si>
+    <t>['11.2.1']</t>
+  </si>
+  <si>
+    <t>['11.3.1', '11.3.2']</t>
+  </si>
+  <si>
+    <t>['11.4.1']</t>
+  </si>
+  <si>
+    <t>['11.5.1', '11.5.2']</t>
+  </si>
+  <si>
+    <t>['11.6.1', '11.6.2']</t>
+  </si>
+  <si>
+    <t>['11.7.1', '11.7.2']</t>
+  </si>
+  <si>
+    <t>['11.a.1']</t>
+  </si>
+  <si>
+    <t>['11.b.1', '11.b.2']</t>
+  </si>
+  <si>
+    <t>['12.1.1']</t>
+  </si>
+  <si>
+    <t>['12.2.1', '12.2.2']</t>
+  </si>
+  <si>
+    <t>['12.3.1']</t>
+  </si>
+  <si>
+    <t>['12.4.1', '12.4.2']</t>
+  </si>
+  <si>
+    <t>['12.5.1']</t>
+  </si>
+  <si>
+    <t>['12.6.1']</t>
+  </si>
+  <si>
+    <t>['12.7.1']</t>
+  </si>
+  <si>
+    <t>['12.8.1']</t>
+  </si>
+  <si>
+    <t>['12.a.1']</t>
+  </si>
+  <si>
+    <t>['12.b.1']</t>
+  </si>
+  <si>
+    <t>['12.c.1']</t>
+  </si>
+  <si>
+    <t>['13.1.1', '13.1.2', '13.1.3']</t>
+  </si>
+  <si>
+    <t>['13.2.1', '13.2.2']</t>
+  </si>
+  <si>
+    <t>['13.3.1']</t>
+  </si>
+  <si>
+    <t>['13.a.1']</t>
+  </si>
+  <si>
+    <t>['13.b.1']</t>
+  </si>
+  <si>
+    <t>['14.1.1']</t>
+  </si>
+  <si>
+    <t>['14.2.1']</t>
+  </si>
+  <si>
+    <t>['14.3.1']</t>
+  </si>
+  <si>
+    <t>['14.4.1']</t>
+  </si>
+  <si>
+    <t>['14.5.1']</t>
+  </si>
+  <si>
+    <t>['14.6.1']</t>
+  </si>
+  <si>
+    <t>['14.7.1']</t>
+  </si>
+  <si>
+    <t>['14.a.1']</t>
+  </si>
+  <si>
+    <t>['14.b.1']</t>
+  </si>
+  <si>
+    <t>['14.c.1']</t>
+  </si>
+  <si>
+    <t>['15.1.1', '15.1.2']</t>
+  </si>
+  <si>
+    <t>['15.2.1']</t>
+  </si>
+  <si>
+    <t>['15.3.1']</t>
+  </si>
+  <si>
+    <t>['15.4.1', '15.4.2']</t>
+  </si>
+  <si>
+    <t>['15.5.1']</t>
+  </si>
+  <si>
+    <t>['15.6.1']</t>
+  </si>
+  <si>
+    <t>['15.7.1']</t>
+  </si>
+  <si>
+    <t>['15.8.1']</t>
+  </si>
+  <si>
+    <t>['15.9.1']</t>
+  </si>
+  <si>
+    <t>['15.a.1']</t>
+  </si>
+  <si>
+    <t>['15.b.1']</t>
+  </si>
+  <si>
+    <t>['15.c.1']</t>
+  </si>
+  <si>
+    <t>['16.1.1', '16.1.2', '16.1.3', '16.1.4']</t>
+  </si>
+  <si>
+    <t>['16.10.1', '16.10.2']</t>
+  </si>
+  <si>
+    <t>['16.2.1', '16.2.2', '16.2.3']</t>
+  </si>
+  <si>
+    <t>['16.3.1', '16.3.2', '16.3.3']</t>
+  </si>
+  <si>
+    <t>['16.4.1', '16.4.2']</t>
+  </si>
+  <si>
+    <t>['16.5.1', '16.5.2']</t>
+  </si>
+  <si>
+    <t>['16.6.1', '16.6.2']</t>
+  </si>
+  <si>
+    <t>['16.7.1', '16.7.2']</t>
+  </si>
+  <si>
+    <t>['16.8.1']</t>
+  </si>
+  <si>
+    <t>['16.9.1']</t>
+  </si>
+  <si>
+    <t>['16.a.1']</t>
+  </si>
+  <si>
+    <t>['16.b.1']</t>
+  </si>
+  <si>
+    <t>['17.1.1', '17.1.2']</t>
+  </si>
+  <si>
+    <t>['17.10.1']</t>
+  </si>
+  <si>
+    <t>['17.11.1']</t>
+  </si>
+  <si>
+    <t>['17.12.1']</t>
+  </si>
+  <si>
+    <t>['17.13.1']</t>
+  </si>
+  <si>
+    <t>['17.14.1']</t>
+  </si>
+  <si>
+    <t>['17.15.1']</t>
+  </si>
+  <si>
+    <t>['17.16.1']</t>
+  </si>
+  <si>
+    <t>['17.17.1']</t>
+  </si>
+  <si>
+    <t>['17.18.1', '17.18.2', '17.18.3']</t>
+  </si>
+  <si>
+    <t>['17.19.1', '17.19.2']</t>
+  </si>
+  <si>
+    <t>['17.2.1']</t>
+  </si>
+  <si>
+    <t>['17.3.1', '17.3.2']</t>
+  </si>
+  <si>
+    <t>['17.4.1']</t>
+  </si>
+  <si>
+    <t>['17.5.1']</t>
+  </si>
+  <si>
+    <t>['17.6.1']</t>
+  </si>
+  <si>
+    <t>['17.7.1']</t>
+  </si>
+  <si>
+    <t>['17.8.1']</t>
+  </si>
+  <si>
+    <t>['17.9.1']</t>
+  </si>
+  <si>
+    <t>16.10</t>
+  </si>
+  <si>
+    <t>17.10</t>
+  </si>
+  <si>
+    <t>17.11</t>
+  </si>
+  <si>
+    <t>17.12</t>
+  </si>
+  <si>
+    <t>17.13</t>
+  </si>
+  <si>
+    <t>17.14</t>
+  </si>
+  <si>
+    <t>17.15</t>
+  </si>
+  <si>
+    <t>17.16</t>
+  </si>
+  <si>
+    <t>17.17</t>
+  </si>
+  <si>
+    <t>17.18</t>
+  </si>
+  <si>
+    <t>17.19</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B187"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1527,7 +1563,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1535,10 +1574,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>232</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,10 +1585,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,10 +1596,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>234</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,10 +1618,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>236</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,10 +1629,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1601,10 +1640,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1612,7 +1651,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>237</v>
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1620,10 +1662,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1631,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,10 +1684,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,10 +1695,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>241</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1664,10 +1706,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>242</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,10 +1717,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1686,10 +1728,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>191</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1697,10 +1739,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>192</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,7 +1750,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>243</v>
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,10 +1761,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>244</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1727,10 +1772,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>245</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1738,10 +1783,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>246</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,10 +1794,10 @@
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>247</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1760,10 +1805,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1771,10 +1816,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>249</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1782,10 +1827,10 @@
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>250</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,10 +1838,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>251</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,10 +1849,10 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>252</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,10 +1860,10 @@
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>193</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,10 +1871,10 @@
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,10 +1882,10 @@
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,10 +1893,10 @@
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1859,7 +1904,10 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>253</v>
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,10 +1915,10 @@
         <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>254</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,10 +1926,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>255</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,10 +1937,10 @@
         <v>13</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>256</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,10 +1948,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,10 +1959,10 @@
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>258</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1922,10 +1970,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>259</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,10 +1981,10 @@
         <v>13</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>260</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1944,10 +1992,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>197</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1955,10 +2003,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,10 +2014,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>199</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,7 +2025,10 @@
         <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>261</v>
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1985,10 +2036,10 @@
         <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>262</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1996,10 +2047,10 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>263</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2007,10 +2058,10 @@
         <v>14</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>264</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2018,10 +2069,10 @@
         <v>14</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>265</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2029,10 +2080,10 @@
         <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>266</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2040,10 +2091,10 @@
         <v>14</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>267</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2051,10 +2102,10 @@
         <v>14</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2062,10 +2113,10 @@
         <v>14</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2073,10 +2124,10 @@
         <v>14</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>202</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>153</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2084,7 +2135,10 @@
         <v>15</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>268</v>
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,10 +2146,10 @@
         <v>15</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>269</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,10 +2157,10 @@
         <v>15</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>270</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,10 +2168,10 @@
         <v>15</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>271</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,10 +2179,10 @@
         <v>15</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,10 +2190,10 @@
         <v>15</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>273</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2147,10 +2201,10 @@
         <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>274</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,10 +2212,10 @@
         <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,10 +2223,10 @@
         <v>15</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>204</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2234,10 @@
         <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>275</v>
+        <v>106</v>
+      </c>
+      <c r="C63" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,10 +2245,10 @@
         <v>16</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>276</v>
+        <v>107</v>
       </c>
       <c r="C64" t="s">
-        <v>162</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,10 +2256,10 @@
         <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>277</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2210,10 +2267,10 @@
         <v>16</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>278</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>164</v>
+        <v>252</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2221,10 +2278,10 @@
         <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>205</v>
+        <v>36</v>
       </c>
       <c r="C67" t="s">
-        <v>165</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2232,10 +2289,10 @@
         <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>206</v>
+        <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>166</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,7 +2300,10 @@
         <v>17</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>279</v>
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2251,10 +2311,10 @@
         <v>17</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>280</v>
+        <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2262,10 +2322,10 @@
         <v>17</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>280</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>168</v>
+        <v>256</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2273,10 +2333,10 @@
         <v>17</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>281</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2284,10 +2344,10 @@
         <v>17</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>282</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2295,10 +2355,10 @@
         <v>17</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>283</v>
+        <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2306,10 +2366,10 @@
         <v>17</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>284</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2317,10 +2377,10 @@
         <v>17</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>285</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>173</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2328,10 +2388,10 @@
         <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>286</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>174</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2339,10 +2399,10 @@
         <v>17</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>287</v>
+        <v>118</v>
       </c>
       <c r="C78" t="s">
-        <v>175</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,10 +2410,10 @@
         <v>17</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>288</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,10 +2421,10 @@
         <v>17</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>207</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2372,10 +2432,10 @@
         <v>17</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>208</v>
+        <v>39</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,7 +2443,10 @@
         <v>18</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>289</v>
+        <v>120</v>
+      </c>
+      <c r="C82" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2391,10 +2454,10 @@
         <v>18</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>290</v>
+        <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2402,10 +2465,10 @@
         <v>18</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>291</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>268</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2413,10 +2476,10 @@
         <v>18</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
       <c r="C85" t="s">
-        <v>181</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2424,10 +2487,10 @@
         <v>18</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>293</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2435,10 +2498,10 @@
         <v>18</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>294</v>
+        <v>125</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2446,10 +2509,10 @@
         <v>18</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,10 +2520,10 @@
         <v>18</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="C89" t="s">
-        <v>185</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2468,10 +2531,10 @@
         <v>18</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
-        <v>186</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2479,7 +2542,10 @@
         <v>3</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>295</v>
+        <v>126</v>
+      </c>
+      <c r="C91" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,10 +2553,10 @@
         <v>3</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>296</v>
+        <v>127</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2498,10 +2564,10 @@
         <v>3</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>297</v>
+        <v>128</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>276</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2509,10 +2575,10 @@
         <v>3</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>298</v>
+        <v>129</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>277</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2520,10 +2586,10 @@
         <v>3</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>299</v>
+        <v>130</v>
       </c>
       <c r="C95" t="s">
-        <v>29</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2531,10 +2597,10 @@
         <v>3</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>300</v>
+        <v>131</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2542,10 +2608,10 @@
         <v>3</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>301</v>
+        <v>132</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>280</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,10 +2619,10 @@
         <v>3</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>302</v>
+        <v>133</v>
       </c>
       <c r="C98" t="s">
-        <v>32</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2564,10 +2630,10 @@
         <v>3</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>212</v>
+        <v>43</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2575,10 +2641,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2586,10 +2652,10 @@
         <v>3</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>214</v>
+        <v>45</v>
       </c>
       <c r="C101" t="s">
-        <v>35</v>
+        <v>284</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2597,7 +2663,10 @@
         <v>4</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>303</v>
+        <v>134</v>
+      </c>
+      <c r="C102" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,10 +2674,10 @@
         <v>4</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>304</v>
+        <v>135</v>
       </c>
       <c r="C103" t="s">
-        <v>36</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,10 +2685,10 @@
         <v>4</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>305</v>
+        <v>136</v>
       </c>
       <c r="C104" t="s">
-        <v>37</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,10 +2696,10 @@
         <v>4</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>306</v>
+        <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>38</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2707,10 @@
         <v>4</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>307</v>
+        <v>138</v>
       </c>
       <c r="C106" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,10 +2718,10 @@
         <v>4</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>308</v>
+        <v>139</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,10 +2729,10 @@
         <v>4</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>309</v>
+        <v>140</v>
       </c>
       <c r="C108" t="s">
-        <v>41</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,10 +2740,10 @@
         <v>4</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>310</v>
+        <v>141</v>
       </c>
       <c r="C109" t="s">
-        <v>42</v>
+        <v>291</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,10 +2751,10 @@
         <v>4</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>215</v>
+        <v>46</v>
       </c>
       <c r="C110" t="s">
-        <v>43</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,10 +2762,10 @@
         <v>4</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>216</v>
+        <v>47</v>
       </c>
       <c r="C111" t="s">
-        <v>44</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2704,7 +2773,10 @@
         <v>4</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>217</v>
+        <v>48</v>
+      </c>
+      <c r="C112" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2712,7 +2784,10 @@
         <v>5</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>311</v>
+        <v>142</v>
+      </c>
+      <c r="C113" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2720,10 +2795,10 @@
         <v>5</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>312</v>
+        <v>143</v>
       </c>
       <c r="C114" t="s">
-        <v>45</v>
+        <v>294</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2731,10 +2806,10 @@
         <v>5</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>313</v>
+        <v>144</v>
       </c>
       <c r="C115" t="s">
-        <v>46</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2742,10 +2817,10 @@
         <v>5</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>314</v>
+        <v>145</v>
       </c>
       <c r="C116" t="s">
-        <v>47</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2753,10 +2828,10 @@
         <v>5</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>315</v>
+        <v>146</v>
       </c>
       <c r="C117" t="s">
-        <v>48</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2764,10 +2839,10 @@
         <v>5</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>316</v>
+        <v>147</v>
       </c>
       <c r="C118" t="s">
-        <v>49</v>
+        <v>298</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -2775,10 +2850,10 @@
         <v>5</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>317</v>
+        <v>148</v>
       </c>
       <c r="C119" t="s">
-        <v>50</v>
+        <v>299</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2786,10 +2861,10 @@
         <v>5</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>318</v>
+        <v>149</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>300</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2797,10 +2872,10 @@
         <v>5</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>319</v>
+        <v>150</v>
       </c>
       <c r="C121" t="s">
-        <v>52</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -2808,10 +2883,10 @@
         <v>5</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>218</v>
+        <v>49</v>
       </c>
       <c r="C122" t="s">
-        <v>53</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -2819,10 +2894,10 @@
         <v>5</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>219</v>
+        <v>50</v>
       </c>
       <c r="C123" t="s">
-        <v>54</v>
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -2830,10 +2905,10 @@
         <v>5</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="C124" t="s">
-        <v>55</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -2841,7 +2916,10 @@
         <v>6</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>320</v>
+        <v>151</v>
+      </c>
+      <c r="C125" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -2849,10 +2927,10 @@
         <v>6</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>321</v>
+        <v>152</v>
       </c>
       <c r="C126" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2860,10 +2938,10 @@
         <v>6</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>322</v>
+        <v>153</v>
       </c>
       <c r="C127" t="s">
-        <v>57</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2871,10 +2949,10 @@
         <v>6</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>323</v>
+        <v>154</v>
       </c>
       <c r="C128" t="s">
-        <v>58</v>
+        <v>307</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2882,10 +2960,10 @@
         <v>6</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>221</v>
+        <v>52</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>308</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2893,10 +2971,10 @@
         <v>6</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>222</v>
+        <v>53</v>
       </c>
       <c r="C130" t="s">
-        <v>60</v>
+        <v>309</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2904,7 +2982,10 @@
         <v>7</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>324</v>
+        <v>155</v>
+      </c>
+      <c r="C131" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2912,10 +2993,10 @@
         <v>7</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>325</v>
+        <v>156</v>
       </c>
       <c r="C132" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,10 +3004,10 @@
         <v>7</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>326</v>
+        <v>157</v>
       </c>
       <c r="C133" t="s">
-        <v>62</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2934,10 +3015,10 @@
         <v>7</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>327</v>
+        <v>158</v>
       </c>
       <c r="C134" t="s">
-        <v>63</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2945,10 +3026,10 @@
         <v>7</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>328</v>
+        <v>159</v>
       </c>
       <c r="C135" t="s">
-        <v>64</v>
+        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2956,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>329</v>
+        <v>160</v>
       </c>
       <c r="C136" t="s">
-        <v>65</v>
+        <v>314</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2967,10 +3048,10 @@
         <v>7</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>330</v>
+        <v>161</v>
       </c>
       <c r="C137" t="s">
-        <v>66</v>
+        <v>315</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2978,10 +3059,10 @@
         <v>7</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>331</v>
+        <v>162</v>
       </c>
       <c r="C138" t="s">
-        <v>67</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2989,10 +3070,10 @@
         <v>7</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="C139" t="s">
-        <v>68</v>
+        <v>317</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3000,10 +3081,10 @@
         <v>7</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>224</v>
+        <v>55</v>
       </c>
       <c r="C140" t="s">
-        <v>69</v>
+        <v>318</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -3011,10 +3092,10 @@
         <v>7</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>225</v>
+        <v>56</v>
       </c>
       <c r="C141" t="s">
-        <v>70</v>
+        <v>319</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -3022,7 +3103,10 @@
         <v>8</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>332</v>
+        <v>163</v>
+      </c>
+      <c r="C142" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -3030,10 +3114,10 @@
         <v>8</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>333</v>
+        <v>164</v>
       </c>
       <c r="C143" t="s">
-        <v>71</v>
+        <v>320</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -3041,10 +3125,10 @@
         <v>8</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>334</v>
+        <v>165</v>
       </c>
       <c r="C144" t="s">
-        <v>72</v>
+        <v>321</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3052,10 +3136,10 @@
         <v>8</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>335</v>
+        <v>166</v>
       </c>
       <c r="C145" t="s">
-        <v>73</v>
+        <v>322</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3063,10 +3147,10 @@
         <v>8</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>336</v>
+        <v>167</v>
       </c>
       <c r="C146" t="s">
-        <v>74</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3074,10 +3158,10 @@
         <v>8</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>337</v>
+        <v>168</v>
       </c>
       <c r="C147" t="s">
-        <v>75</v>
+        <v>324</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3085,10 +3169,10 @@
         <v>8</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>338</v>
+        <v>169</v>
       </c>
       <c r="C148" t="s">
-        <v>76</v>
+        <v>325</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3096,10 +3180,10 @@
         <v>8</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>339</v>
+        <v>170</v>
       </c>
       <c r="C149" t="s">
-        <v>77</v>
+        <v>326</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3107,10 +3191,10 @@
         <v>8</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>340</v>
+        <v>171</v>
       </c>
       <c r="C150" t="s">
-        <v>78</v>
+        <v>327</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3118,10 +3202,10 @@
         <v>8</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>341</v>
+        <v>172</v>
       </c>
       <c r="C151" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3129,10 +3213,10 @@
         <v>8</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>226</v>
+        <v>57</v>
       </c>
       <c r="C152" t="s">
-        <v>80</v>
+        <v>329</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3140,10 +3224,10 @@
         <v>8</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>227</v>
+        <v>58</v>
       </c>
       <c r="C153" t="s">
-        <v>81</v>
+        <v>330</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3151,10 +3235,10 @@
         <v>8</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>228</v>
+        <v>59</v>
       </c>
       <c r="C154" t="s">
-        <v>82</v>
+        <v>331</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3162,7 +3246,10 @@
         <v>9</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>342</v>
+        <v>173</v>
+      </c>
+      <c r="C155" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3170,10 +3257,10 @@
         <v>9</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>343</v>
+        <v>174</v>
       </c>
       <c r="C156" t="s">
-        <v>83</v>
+        <v>332</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,10 +3268,10 @@
         <v>9</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>343</v>
+        <v>175</v>
       </c>
       <c r="C157" t="s">
-        <v>84</v>
+        <v>334</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3192,10 +3279,10 @@
         <v>9</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>344</v>
+        <v>176</v>
       </c>
       <c r="C158" t="s">
-        <v>85</v>
+        <v>335</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,10 +3290,10 @@
         <v>9</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>345</v>
+        <v>177</v>
       </c>
       <c r="C159" t="s">
-        <v>86</v>
+        <v>336</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3214,10 +3301,10 @@
         <v>9</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>346</v>
+        <v>178</v>
       </c>
       <c r="C160" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3225,10 +3312,10 @@
         <v>9</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>347</v>
+        <v>179</v>
       </c>
       <c r="C161" t="s">
-        <v>88</v>
+        <v>338</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3236,10 +3323,10 @@
         <v>9</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>348</v>
+        <v>180</v>
       </c>
       <c r="C162" t="s">
-        <v>89</v>
+        <v>339</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3247,10 +3334,10 @@
         <v>9</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>349</v>
+        <v>181</v>
       </c>
       <c r="C163" t="s">
-        <v>90</v>
+        <v>340</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3258,32 +3345,32 @@
         <v>9</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>350</v>
+        <v>182</v>
       </c>
       <c r="C164" t="s">
-        <v>91</v>
+        <v>341</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>351</v>
+      <c r="B165" t="s">
+        <v>363</v>
       </c>
       <c r="C165" t="s">
-        <v>92</v>
+        <v>333</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>9</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>229</v>
+        <v>10</v>
+      </c>
+      <c r="B166" t="s">
+        <v>60</v>
       </c>
       <c r="C166" t="s">
-        <v>93</v>
+        <v>342</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3291,10 +3378,10 @@
         <v>9</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>230</v>
+        <v>61</v>
       </c>
       <c r="C167" t="s">
-        <v>94</v>
+        <v>343</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,7 +3389,10 @@
         <v>10</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>352</v>
+        <v>183</v>
+      </c>
+      <c r="C168" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,10 +3400,10 @@
         <v>10</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>353</v>
+        <v>184</v>
       </c>
       <c r="C169" t="s">
-        <v>95</v>
+        <v>344</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3321,10 +3411,10 @@
         <v>10</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>353</v>
+        <v>185</v>
       </c>
       <c r="C170" t="s">
-        <v>96</v>
+        <v>355</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,10 +3422,10 @@
         <v>10</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>353</v>
+        <v>186</v>
       </c>
       <c r="C171" t="s">
-        <v>97</v>
+        <v>356</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,10 +3433,10 @@
         <v>10</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>353</v>
+        <v>187</v>
       </c>
       <c r="C172" t="s">
-        <v>98</v>
+        <v>357</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3354,10 +3444,10 @@
         <v>10</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>353</v>
+        <v>188</v>
       </c>
       <c r="C173" t="s">
-        <v>99</v>
+        <v>358</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3365,10 +3455,10 @@
         <v>10</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>353</v>
+        <v>189</v>
       </c>
       <c r="C174" t="s">
-        <v>100</v>
+        <v>359</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3376,10 +3466,10 @@
         <v>10</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>354</v>
+        <v>190</v>
       </c>
       <c r="C175" t="s">
-        <v>101</v>
+        <v>360</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3387,10 +3477,10 @@
         <v>10</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>354</v>
+        <v>191</v>
       </c>
       <c r="C176" t="s">
-        <v>102</v>
+        <v>361</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3398,120 +3488,120 @@
         <v>10</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>354</v>
+        <v>192</v>
       </c>
       <c r="C177" t="s">
-        <v>103</v>
+        <v>362</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>10</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>354</v>
+      <c r="B178" t="s">
+        <v>364</v>
       </c>
       <c r="C178" t="s">
-        <v>104</v>
+        <v>345</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>10</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>354</v>
+      <c r="B179" t="s">
+        <v>365</v>
       </c>
       <c r="C179" t="s">
-        <v>105</v>
+        <v>346</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>10</v>
       </c>
-      <c r="B180" s="1" t="s">
-        <v>354</v>
+      <c r="B180" t="s">
+        <v>366</v>
       </c>
       <c r="C180" t="s">
-        <v>106</v>
+        <v>347</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>10</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>355</v>
+      <c r="B181" t="s">
+        <v>367</v>
       </c>
       <c r="C181" t="s">
-        <v>107</v>
+        <v>348</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>10</v>
       </c>
-      <c r="B182" s="1" t="s">
-        <v>356</v>
+      <c r="B182" t="s">
+        <v>368</v>
       </c>
       <c r="C182" t="s">
-        <v>108</v>
+        <v>349</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>10</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>357</v>
+      <c r="B183" t="s">
+        <v>369</v>
       </c>
       <c r="C183" t="s">
-        <v>109</v>
+        <v>350</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>10</v>
       </c>
-      <c r="B184" s="1" t="s">
-        <v>358</v>
+      <c r="B184" t="s">
+        <v>370</v>
       </c>
       <c r="C184" t="s">
-        <v>110</v>
+        <v>351</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>10</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>359</v>
+      <c r="B185" t="s">
+        <v>371</v>
       </c>
       <c r="C185" t="s">
-        <v>111</v>
+        <v>352</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>10</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>360</v>
+      <c r="B186" t="s">
+        <v>372</v>
       </c>
       <c r="C186" t="s">
-        <v>112</v>
+        <v>353</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>10</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>361</v>
+      <c r="B187" t="s">
+        <v>373</v>
       </c>
       <c r="C187" t="s">
-        <v>113</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SDGS-76 implemented and integrated a prototype for associating targets and indicators. Output saved in both the excel files and in json
</commit_message>
<xml_diff>
--- a/keywords/indicators.xlsx
+++ b/keywords/indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7400AAF-4B80-45E0-9105-8827EEC3AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF30FD9-2B44-40EF-9255-5DD7A9C1440E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="375">
   <si>
     <t>Goal</t>
   </si>
@@ -1153,6 +1153,9 @@
   </si>
   <si>
     <t>17.19</t>
+  </si>
+  <si>
+    <t>8.10</t>
   </si>
 </sst>
 </file>
@@ -1537,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,10 +2325,10 @@
         <v>17</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,10 +2336,10 @@
         <v>17</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,10 +2347,10 @@
         <v>17</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C73" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,10 +2358,10 @@
         <v>17</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C74" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,10 +2369,10 @@
         <v>17</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C75" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,10 +2380,10 @@
         <v>17</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,10 +2391,10 @@
         <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,10 +2402,10 @@
         <v>17</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C78" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2413,10 @@
         <v>17</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>119</v>
+        <v>374</v>
       </c>
       <c r="C79" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>